<commit_message>
update abecip and fgv data
</commit_message>
<xml_diff>
--- a/data-raw/abecip_cgi.xlsx
+++ b/data-raw/abecip_cgi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciusoike/Documents/GitHub/realestatebr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1838884F-CA9F-E541-9069-1AA2C561BD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72AD812-9544-6446-B365-5EC3E24A57C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1280" windowWidth="15920" windowHeight="14880" xr2:uid="{E617B1F6-EB34-2A4E-917E-41F92E27F3C5}"/>
+    <workbookView xWindow="520" yWindow="1180" windowWidth="15920" windowHeight="14880" xr2:uid="{E617B1F6-EB34-2A4E-917E-41F92E27F3C5}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="263">
   <si>
     <t xml:space="preserve">Més </t>
   </si>
@@ -785,6 +785,42 @@
   </si>
   <si>
     <t>18,463,629,282</t>
+  </si>
+  <si>
+    <t>639,169,072.76</t>
+  </si>
+  <si>
+    <t>633,235,924.42</t>
+  </si>
+  <si>
+    <t>711,061,546.22</t>
+  </si>
+  <si>
+    <t>647,341,309.41</t>
+  </si>
+  <si>
+    <t>160.7</t>
+  </si>
+  <si>
+    <t>158.5</t>
+  </si>
+  <si>
+    <t>157.9</t>
+  </si>
+  <si>
+    <t>3.8%</t>
+  </si>
+  <si>
+    <t>18,835,612,488</t>
+  </si>
+  <si>
+    <t>19,035,834,637</t>
+  </si>
+  <si>
+    <t>19.401,421,366</t>
+  </si>
+  <si>
+    <t>19,687,763,253</t>
   </si>
 </sst>
 </file>
@@ -856,9 +892,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -896,7 +932,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1002,7 +1038,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1144,7 +1180,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1155,8 +1191,8 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F76" sqref="F76"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3271,14 +3307,115 @@
         <v>128</v>
       </c>
       <c r="G81" s="1">
-        <v>117.11</v>
+        <v>117110</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>250</v>
       </c>
     </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2023</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D82" s="1">
+        <v>2524</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G82" s="1">
+        <v>118252</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>2023</v>
+      </c>
+      <c r="B83" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D83" s="1">
+        <v>2399</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G83" s="1">
+        <v>118894</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>2023</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D84" s="1">
+        <v>2760</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G84" s="1">
+        <v>120052</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C85" s="1"/>
+      <c r="A85">
+        <v>2023</v>
+      </c>
+      <c r="B85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D85" s="1">
+        <v>2409</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G85" s="1">
+        <v>120833</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C86" s="1"/>
@@ -3300,26 +3437,22 @@
       <c r="C90" s="1"/>
       <c r="E90" s="1"/>
       <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C91" s="1"/>
       <c r="E91" s="1"/>
       <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C92" s="1"/>
       <c r="E92" s="1"/>
       <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C93" s="1"/>
       <c r="E93" s="1"/>
       <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>